<commit_message>
Noch ein paar Infos zu den ERF hinzugefügt
</commit_message>
<xml_diff>
--- a/data/functionsETCHE.xlsx
+++ b/data/functionsETCHE.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lochmannm\Documents\GitHub\Healthiar_Sandbox\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lochmannm\Documents\GitHub\Hessen_END_Healthiar\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{860DBB59-5E8A-4DA7-8BCD-D2B0893C8B7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A262D3FA-C83F-4EAF-AB37-6FE9E5EE4C4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-1980" windowWidth="29040" windowHeight="17520" xr2:uid="{48A8F245-2396-4F0B-B734-4CFAEB6227B4}"/>
   </bookViews>
@@ -153,9 +153,6 @@
     <t>1 - abs(72 - (-90.70 + c * 1.80) / sqrt(1789 + 272))</t>
   </si>
   <si>
-    <t>ifelse (c &gt;= threshold, 1 / (1 + exp(-(log(0.1 / 0.9) + (log(1.38) / 10 * (c - 50))))), 0.1)</t>
-  </si>
-  <si>
     <t>ifelse(c&gt;threshold,(c-threshold)*1.055,0)</t>
   </si>
   <si>
@@ -187,6 +184,9 @@
   </si>
   <si>
     <t>0.006</t>
+  </si>
+  <si>
+    <t>100*ifelse (c &gt;= threshold, 1 / (1 + exp(-(log(0.1 / 0.9) + (log(1.38) / 10 * (c - 50))))), 0.1)</t>
   </si>
 </sst>
 </file>
@@ -255,7 +255,7 @@
       <xdr:col>24</xdr:col>
       <xdr:colOff>153755</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>87021</xdr:rowOff>
+      <xdr:rowOff>83846</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -299,7 +299,7 @@
       <xdr:col>10</xdr:col>
       <xdr:colOff>686177</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>62449</xdr:rowOff>
+      <xdr:rowOff>65624</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -324,6 +324,50 @@
         <a:xfrm>
           <a:off x="1466272" y="4271818"/>
           <a:ext cx="6839905" cy="2810267"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>521724</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>133482</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Grafik 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{33D87F0E-630E-464B-8C2F-109C6CB6475E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="47625" y="7153275"/>
+          <a:ext cx="7335274" cy="943107"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -634,8 +678,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8156CAC4-1F63-4625-9494-276B4F46068B}">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -645,13 +689,13 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C1" t="s">
         <v>33</v>
       </c>
       <c r="D1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
@@ -669,7 +713,7 @@
         <v>34</v>
       </c>
       <c r="J1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
@@ -677,7 +721,7 @@
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C2" t="s">
         <v>29</v>
@@ -694,11 +738,14 @@
       <c r="G2" t="s">
         <v>3</v>
       </c>
+      <c r="H2">
+        <v>45</v>
+      </c>
       <c r="I2" t="s">
         <v>0</v>
       </c>
       <c r="J2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
@@ -706,7 +753,7 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C3" t="s">
         <v>29</v>
@@ -723,11 +770,14 @@
       <c r="G3" t="s">
         <v>3</v>
       </c>
+      <c r="H3">
+        <v>45</v>
+      </c>
       <c r="I3" t="s">
         <v>0</v>
       </c>
       <c r="J3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
@@ -735,7 +785,7 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C4" t="s">
         <v>29</v>
@@ -752,11 +802,14 @@
       <c r="G4" t="s">
         <v>3</v>
       </c>
+      <c r="H4">
+        <v>45</v>
+      </c>
       <c r="I4" t="s">
         <v>0</v>
       </c>
       <c r="J4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
@@ -764,7 +817,7 @@
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C5" t="s">
         <v>29</v>
@@ -781,11 +834,14 @@
       <c r="G5" t="s">
         <v>3</v>
       </c>
+      <c r="H5">
+        <v>45</v>
+      </c>
       <c r="I5" t="s">
         <v>15</v>
       </c>
       <c r="J5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
@@ -793,7 +849,7 @@
         <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C6" t="s">
         <v>29</v>
@@ -810,11 +866,14 @@
       <c r="G6" t="s">
         <v>4</v>
       </c>
+      <c r="H6">
+        <v>40</v>
+      </c>
       <c r="I6" t="s">
         <v>18</v>
       </c>
       <c r="J6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
@@ -822,7 +881,7 @@
         <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C7" t="s">
         <v>29</v>
@@ -839,11 +898,14 @@
       <c r="G7" t="s">
         <v>4</v>
       </c>
+      <c r="H7">
+        <v>40</v>
+      </c>
       <c r="I7" t="s">
         <v>18</v>
       </c>
       <c r="J7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
@@ -851,7 +913,7 @@
         <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C8" t="s">
         <v>29</v>
@@ -868,11 +930,14 @@
       <c r="G8" t="s">
         <v>4</v>
       </c>
+      <c r="H8">
+        <v>40</v>
+      </c>
       <c r="I8" t="s">
         <v>18</v>
       </c>
       <c r="J8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
@@ -880,7 +945,7 @@
         <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C9" t="s">
         <v>29</v>
@@ -897,11 +962,14 @@
       <c r="G9" t="s">
         <v>4</v>
       </c>
+      <c r="H9">
+        <v>40</v>
+      </c>
       <c r="I9" t="s">
         <v>15</v>
       </c>
       <c r="J9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
@@ -909,7 +977,7 @@
         <v>32</v>
       </c>
       <c r="B10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C10" t="s">
         <v>30</v>
@@ -921,7 +989,7 @@
         <v>5</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G10" t="s">
         <v>3</v>
@@ -938,7 +1006,7 @@
         <v>32</v>
       </c>
       <c r="B11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C11" t="s">
         <v>30</v>
@@ -950,7 +1018,7 @@
         <v>6</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G11" t="s">
         <v>3</v>
@@ -967,7 +1035,7 @@
         <v>32</v>
       </c>
       <c r="B12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C12" t="s">
         <v>30</v>
@@ -979,7 +1047,7 @@
         <v>7</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G12" t="s">
         <v>3</v>
@@ -996,7 +1064,7 @@
         <v>23</v>
       </c>
       <c r="B13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C13" t="s">
         <v>30</v>
@@ -1008,7 +1076,7 @@
         <v>5</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G13" t="s">
         <v>3</v>
@@ -1025,7 +1093,7 @@
         <v>23</v>
       </c>
       <c r="B14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C14" t="s">
         <v>30</v>
@@ -1037,7 +1105,7 @@
         <v>6</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G14" t="s">
         <v>3</v>
@@ -1054,7 +1122,7 @@
         <v>23</v>
       </c>
       <c r="B15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C15" t="s">
         <v>30</v>
@@ -1066,7 +1134,7 @@
         <v>7</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G15" t="s">
         <v>3</v>
@@ -1083,7 +1151,7 @@
         <v>25</v>
       </c>
       <c r="B16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C16" t="s">
         <v>30</v>
@@ -1095,7 +1163,7 @@
         <v>5</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G16" t="s">
         <v>3</v>
@@ -1112,7 +1180,7 @@
         <v>25</v>
       </c>
       <c r="B17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C17" t="s">
         <v>30</v>
@@ -1124,7 +1192,7 @@
         <v>6</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G17" t="s">
         <v>3</v>
@@ -1141,7 +1209,7 @@
         <v>25</v>
       </c>
       <c r="B18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C18" t="s">
         <v>30</v>
@@ -1153,7 +1221,7 @@
         <v>7</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G18" t="s">
         <v>3</v>
@@ -1170,7 +1238,7 @@
         <v>27</v>
       </c>
       <c r="B19" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C19" t="s">
         <v>29</v>
@@ -1182,7 +1250,7 @@
         <v>7</v>
       </c>
       <c r="F19" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="G19" t="s">
         <v>3</v>
@@ -1194,7 +1262,7 @@
         <v>28</v>
       </c>
       <c r="J19" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>